<commit_message>
upcountry changes in job card
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/BookingJobCard_Template-v8.xlsx
+++ b/application/controllers/excel-templates/BookingJobCard_Template-v8.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-dev/application/controllers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>247AROUND SERVICE JOB CARD</t>
   </si>
@@ -168,6 +168,13 @@
   </si>
   <si>
     <t>Rating (1-5)</t>
+  </si>
+  <si>
+    <t>Upcountry
+Charges</t>
+  </si>
+  <si>
+    <t>{booking:upcountry_charges}</t>
   </si>
 </sst>
 </file>
@@ -639,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -749,6 +756,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -789,14 +817,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -815,32 +849,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1168,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G23"/>
+  <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1201,79 +1223,79 @@
     </row>
     <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="23"/>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="52"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="2:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="2:7" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="41"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="45"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="52"/>
     </row>
     <row r="9" spans="2:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
@@ -1285,15 +1307,15 @@
       <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="47"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:7" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="27" t="s">
         <v>18</v>
       </c>
@@ -1303,10 +1325,10 @@
       <c r="D10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="49"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="34" t="s">
         <v>22</v>
       </c>
@@ -1324,68 +1346,70 @@
       <c r="E11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
+    <row r="13" spans="2:7" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C13" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
-    </row>
-    <row r="13" spans="2:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="25" t="s">
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+    </row>
+    <row r="14" spans="2:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="28" t="s">
+      <c r="C14" s="60"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="29">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B16" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -1394,85 +1418,107 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B17" s="30">
+      <c r="B17" s="29">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" s="30">
         <v>3</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="2:7" ht="22" x14ac:dyDescent="0.15">
-      <c r="B18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="17" t="s">
-        <v>27</v>
-      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
     <row r="19" spans="2:7" ht="22" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" ht="22" x14ac:dyDescent="0.15">
+      <c r="B20" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="36" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="31" t="s">
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="17" t="s">
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="2:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="31" t="s">
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="17" t="s">
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="37" t="s">
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="32"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19" t="s">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="46"/>
+    </row>
+    <row r="24" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="32"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="20"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:G8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="C3:G3"/>
@@ -1480,17 +1526,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:G8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>